<commit_message>
Updated Scorecard by Cyan & Patricia
</commit_message>
<xml_diff>
--- a/04-Software-Testing/UPSMS-Scorecard.xlsx
+++ b/04-Software-Testing/UPSMS-Scorecard.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan V\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="Signatory" sheetId="2" r:id="rId2"/>
+    <sheet name="Admin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Use Case</t>
   </si>
@@ -45,12 +50,6 @@
     <t>View Scholarship Status</t>
   </si>
   <si>
-    <t>Update Profile</t>
-  </si>
-  <si>
-    <t>Review Accomplishments</t>
-  </si>
-  <si>
     <t>Successful log-in (user)</t>
   </si>
   <si>
@@ -84,36 +83,12 @@
     <t>Error message: Invalid username/password</t>
   </si>
   <si>
-    <t>User forms will appear</t>
-  </si>
-  <si>
-    <t>View Scholarship Status page</t>
-  </si>
-  <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
-    <t>1.1.2</t>
-  </si>
-  <si>
-    <t>Basic Flow (Student submits changes to his/her profile)</t>
-  </si>
-  <si>
     <t>Prototype: Returns to homepage; System: Updates database, pop-up message: Edit Successful!</t>
   </si>
   <si>
-    <t>Student cancels the changes to his/her profile</t>
-  </si>
-  <si>
     <t>Prototype: Returns to homepage; System: Forms now contain original information</t>
   </si>
   <si>
-    <t>User homepage &gt; User Profile &gt; Edit User Profile</t>
-  </si>
-  <si>
-    <t>User homepage &gt; View Scholarship Status button</t>
-  </si>
-  <si>
     <t>User homepage &gt; User Profile &gt; Edit User Profile &gt; User edits information &gt; Submit</t>
   </si>
   <si>
@@ -123,37 +98,124 @@
     <t>If the application form or supporting documents are not complete</t>
   </si>
   <si>
-    <t>Admin homepage &gt; Applications &gt; See Status &gt; Notify</t>
-  </si>
-  <si>
     <t>Student meets all requirements</t>
   </si>
   <si>
-    <t>Admin homepage &gt; Applications &gt; See Status &gt; Accept</t>
-  </si>
-  <si>
     <t>If the student does not meet all the specified requirements for a grant</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin homepage &gt; Applications &gt; See Status &gt; Reject </t>
-  </si>
-  <si>
-    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Accomplishment Report</t>
-  </si>
-  <si>
-    <t>Review Financial Reports</t>
-  </si>
-  <si>
-    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Financial Report</t>
-  </si>
-  <si>
     <t>Prototype: Do nothing; System: Notify student, update database</t>
   </si>
   <si>
-    <t>Prototype: Do nothing; System: Retain/Remove scholarship or Warn student, update database</t>
-  </si>
-  <si>
-    <t>Prototype: Do nothing; System: Grant/Do not grant financial assistance, update database</t>
+    <t>Prototype: Do nothing; System: If all signatures are complete: notify admin; else: pass to next signatory; update database</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Notify admin, update database</t>
+  </si>
+  <si>
+    <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Accept</t>
+  </si>
+  <si>
+    <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Return</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Return application to applicant/to previous signatory for review, update database</t>
+  </si>
+  <si>
+    <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Reject</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Application &gt; See Status &gt; Accept</t>
+  </si>
+  <si>
+    <t>Once the signatories are done filtering applicants, the admin will accept eligible applicants</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Application &gt; See Status &gt; Reject</t>
+  </si>
+  <si>
+    <t>Once the signatories are done filtering applicants, the admin will reject ineligible applicants</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Accomplishment Report &gt; Keep Scholarship</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Retain Scholarship, update database</t>
+  </si>
+  <si>
+    <t>Review Accomplishments and the User's Scholarship will continue.</t>
+  </si>
+  <si>
+    <t>Review Accomplishments and the User will be warned to improve his study. User's Scholarship will continue.</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Accomplishment Report &gt; Warn Grantee</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Retain Scholarship, update database (number of warnings + 1)</t>
+  </si>
+  <si>
+    <t>Review Accomplishments and the User's Scholarship will be removed.</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Accomplishment Report &gt; Remove Scholarhip</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Remove Scholarship, Update Database, Notify User</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Financial Report &gt; Send Financial Assistance</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Grant financial assistance, update database</t>
+  </si>
+  <si>
+    <t>Review Financial Reports and the User will receive Financial Assistance.</t>
+  </si>
+  <si>
+    <t>Review Financial Reports and the User will not receive Financial Assistance.</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Do not grant financial assistance, update database</t>
+  </si>
+  <si>
+    <t>Admin homepage &gt; Scholarships &gt; View Grantees &gt; Name of Grantee &gt; Financial Report &gt; Reply to User (confirmation of received report)</t>
+  </si>
+  <si>
+    <t>User Profile: Student submits changes to his/her profile</t>
+  </si>
+  <si>
+    <t>User Profile: Student cancels the changes to his/her profile</t>
+  </si>
+  <si>
+    <t>Apply for Scholarship</t>
+  </si>
+  <si>
+    <t>User homepage &gt; Apply for Scholarship &gt; Choose Scholarship &gt; Download Application Form</t>
+  </si>
+  <si>
+    <t>Prototype: Downloads the MOVE UP Form; System: Downloads the correct form depending on the selected scholarship.</t>
+  </si>
+  <si>
+    <t>User homepage &gt; View Scholarship Status</t>
+  </si>
+  <si>
+    <t>Submit Accomplishments Form</t>
+  </si>
+  <si>
+    <t>Prototype &amp; System: Show Scholarship Status (Accepted/Rejected/Pending)</t>
+  </si>
+  <si>
+    <t>Prototype: Do nothing; System: Update database</t>
+  </si>
+  <si>
+    <t>User homepage &gt; Accomplishments Form &gt; Submit</t>
+  </si>
+  <si>
+    <t>Submit Financial Reports</t>
+  </si>
+  <si>
+    <t>User homepage &gt; Financial Reports &gt; Submit</t>
   </si>
 </sst>
 </file>
@@ -213,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +289,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +304,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -284,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,7 +390,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,15 +601,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="27.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
-    <col min="5" max="7" width="27.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="27.140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -576,225 +648,160 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>1.2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
+      <c r="B5" s="2">
+        <v>2.2000000000000002</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
       <c r="B8" s="2">
-        <v>2.2999999999999998</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>3.1</v>
+        <v>6.1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2">
-        <v>5.3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4">
-        <v>5.4</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
@@ -806,24 +813,323 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited scorecard, sig.php, agile estimates
- Signatory account can now filter out applications in the interface. Consideration of Signatory order still not implemented.
- Edited Agile Estimates
</commit_message>
<xml_diff>
--- a/04-Software-Testing/UPSMS-Scorecard.xlsx
+++ b/04-Software-Testing/UPSMS-Scorecard.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan V\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan V\Desktop\CS 191 GitHub\04-Software-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Use Case</t>
   </si>
@@ -107,21 +107,12 @@
     <t>Prototype: Do nothing; System: Notify student, update database</t>
   </si>
   <si>
-    <t>Prototype: Do nothing; System: If all signatures are complete: notify admin; else: pass to next signatory; update database</t>
-  </si>
-  <si>
-    <t>Prototype: Do nothing; System: Notify admin, update database</t>
-  </si>
-  <si>
     <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Accept</t>
   </si>
   <si>
     <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Return</t>
   </si>
   <si>
-    <t>Prototype: Do nothing; System: Return application to applicant/to previous signatory for review, update database</t>
-  </si>
-  <si>
     <t>Signatory homepage &gt; Pending Applications &gt; Tick corresponding checkbox &gt; Reject</t>
   </si>
   <si>
@@ -216,6 +207,36 @@
   </si>
   <si>
     <t>User homepage &gt; Financial Reports &gt; Submit</t>
+  </si>
+  <si>
+    <t>If all signatures are complete: notify admin; else: pass to next signatory; update database</t>
+  </si>
+  <si>
+    <t>Return application to applicant/to previous signatory for review, update database</t>
+  </si>
+  <si>
+    <t>Notify admin, update database</t>
+  </si>
+  <si>
+    <t>Monitoring of applications from the Interface</t>
+  </si>
+  <si>
+    <t>Signatory homepage &gt; Pending Applications</t>
+  </si>
+  <si>
+    <t>Select from database and display on the interface.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Signatory order not yet implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Filtering of applications based on the logged on sigID implemented. Filtering of applications based on the status of the application not yet implemented.</t>
   </si>
 </sst>
 </file>
@@ -681,7 +702,7 @@
         <v>2.1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>22</v>
@@ -698,7 +719,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -717,13 +738,13 @@
         <v>3.1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -739,10 +760,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -755,13 +776,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -774,13 +795,13 @@
         <v>6.1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -813,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,13 +915,17 @@
         <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -911,13 +936,17 @@
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -928,13 +957,40 @@
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -945,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1021,10 +1077,10 @@
         <v>2.1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>27</v>
@@ -1037,10 +1093,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>27</v>
@@ -1056,13 +1112,13 @@
         <v>3.1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1072,13 +1128,13 @@
         <v>3.2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1088,13 +1144,13 @@
         <v>3.3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
@@ -1105,13 +1161,13 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.25">
@@ -1119,13 +1175,13 @@
         <v>4.2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes + Uploaded Deliverables
</commit_message>
<xml_diff>
--- a/04-Software-Testing/UPSMS-Scorecard.xlsx
+++ b/04-Software-Testing/UPSMS-Scorecard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Use Case</t>
   </si>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -710,7 +710,9 @@
       <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -727,7 +729,9 @@
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -836,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1001,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1089,9 @@
       <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -1101,7 +1107,9 @@
       <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>